<commit_message>
Added Email Feature for Slips
</commit_message>
<xml_diff>
--- a/Salary_slips_generator.xlsx
+++ b/Salary_slips_generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\1o1_WorkStation\PaySlip Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD2573C-6C02-49C0-B9CA-EE04E3786DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F36AE1E-B82E-4FEB-B410-596A5009FD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6B31D240-CFB6-4A68-8984-7821AB71E774}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>Email</t>
-  </si>
-  <si>
-    <t>Mayank.Kuthar@emulus.co</t>
   </si>
   <si>
     <t>HRA</t>
@@ -132,6 +129,15 @@
   </si>
   <si>
     <t>CYRLA6392B</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>mayank8055neel@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -289,6 +295,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -296,9 +305,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -323,13 +329,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>76199</xdr:rowOff>
@@ -371,13 +377,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
@@ -419,7 +425,7 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -462,7 +468,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -474,6 +480,92 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1B0185B-1993-44DB-8805-25A7DE4EE654}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="1875692"/>
+          <a:ext cx="304800" cy="304801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304799"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17874685-B809-45B2-ABA5-889F406C041B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="2104292"/>
+          <a:ext cx="304800" cy="304799"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304801"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C97BBA1-30AA-4DB2-B120-9771937DDE88}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1742,146 +1834,152 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E45666-7E45-4118-9856-F2CCDA836002}">
   <sheetPr codeName="Sheet28"/>
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="10.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="7.21875" customWidth="1"/>
-    <col min="5" max="13" width="7.77734375" customWidth="1"/>
-    <col min="14" max="14" width="21.5546875" customWidth="1"/>
-    <col min="15" max="15" width="11.21875" customWidth="1"/>
-    <col min="16" max="16" width="23" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" customWidth="1"/>
-    <col min="22" max="22" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="10.21875" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="7.21875" customWidth="1"/>
+    <col min="6" max="14" width="7.77734375" customWidth="1"/>
+    <col min="15" max="15" width="21.5546875" customWidth="1"/>
+    <col min="16" max="16" width="11.21875" customWidth="1"/>
+    <col min="17" max="17" width="23" customWidth="1"/>
+    <col min="18" max="18" width="10.5546875" customWidth="1"/>
+    <col min="23" max="23" width="23.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="5" t="s">
+    <row r="1" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-    </row>
-    <row r="2" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1">
+        <v>50000</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>12000</v>
+      </c>
+      <c r="H3" s="1">
+        <v>7000</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J3" s="1">
+        <v>800</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3000</v>
+      </c>
+      <c r="L3" s="1">
+        <f>E3+F3+G3+H3-I3-J3+K3</f>
+        <v>79200</v>
+      </c>
+      <c r="M3" s="1">
+        <v>22</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="22.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1">
-        <v>50000</v>
-      </c>
-      <c r="E3" s="1">
-        <v>10000</v>
-      </c>
-      <c r="F3" s="1">
-        <v>12000</v>
-      </c>
-      <c r="G3" s="1">
-        <v>7000</v>
-      </c>
-      <c r="H3" s="1">
-        <v>2000</v>
-      </c>
-      <c r="I3" s="1">
-        <v>800</v>
-      </c>
-      <c r="J3" s="1">
-        <v>3000</v>
-      </c>
-      <c r="K3" s="1">
-        <f>D3+E3+F3+G3-H3-I3+J3</f>
-        <v>79200</v>
-      </c>
-      <c r="L3" s="1">
-        <v>22</v>
-      </c>
-      <c r="M3" s="1">
+      <c r="P3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1899,8 +1997,9 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1918,8 +2017,9 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1937,8 +2037,9 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1959,8 +2060,9 @@
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
-    </row>
-    <row r="8" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1978,8 +2080,9 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1997,8 +2100,9 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2016,8 +2120,9 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2035,8 +2140,9 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2054,8 +2160,9 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2073,8 +2180,9 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2092,8 +2200,9 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2111,8 +2220,9 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2130,8 +2240,9 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2149,8 +2260,9 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2168,8 +2280,9 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2187,8 +2300,9 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2206,8 +2320,9 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2225,8 +2340,9 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2244,8 +2360,9 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2263,8 +2380,9 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
-    </row>
-    <row r="24" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2282,8 +2400,9 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
-    </row>
-    <row r="25" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2301,8 +2420,9 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-    </row>
-    <row r="26" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2320,13 +2440,14 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="E1:L1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="P3" r:id="rId1" xr:uid="{70CFE135-E170-435C-AF6E-AD7C8ED1EA0E}"/>
+    <hyperlink ref="Q3" r:id="rId1" xr:uid="{70CFE135-E170-435C-AF6E-AD7C8ED1EA0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>

</xml_diff>